<commit_message>
Update on STS script
</commit_message>
<xml_diff>
--- a/sts_remove_aws_resources/collection_of_key_values.xlsx
+++ b/sts_remove_aws_resources/collection_of_key_values.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cseregy\Desktop\VScode\github\python_test\sts_remove_aws_resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cseregy\Desktop\github_personal\canada\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2967AA90-76B2-4528-9713-2213509FF4DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -24,31 +25,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>random_value123</t>
-  </si>
-  <si>
-    <t>random_value671</t>
-  </si>
-  <si>
-    <t>random_value654</t>
-  </si>
-  <si>
-    <t>random_value666</t>
-  </si>
-  <si>
-    <t>random_value165_s3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>cseregy-test-1</t>
+  </si>
+  <si>
+    <t>column_0</t>
+  </si>
+  <si>
+    <t>column_1</t>
+  </si>
+  <si>
+    <t>resource_name</t>
+  </si>
+  <si>
+    <t>account_number</t>
+  </si>
+  <si>
+    <t>cseregy-test-2</t>
+  </si>
+  <si>
+    <t>5945869c-1517-4c88-b5b2-b8d3fd35b2f4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -72,15 +88,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -357,65 +376,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>616516541843</v>
+      <c r="B3" s="1">
+        <v>341254748130</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>233215615832</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>341254748130</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>894987511975</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>115487563454</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>213454825397</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>616516239541</v>
+        <v>341254748130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>